<commit_message>
Work on excel importer. Read file, parse artNum, have issue in quantity, cannot parse numeric to String.
</commit_message>
<xml_diff>
--- a/Grohe/src/main/resources/test.xlsx
+++ b/Grohe/src/main/resources/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Office\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T480s\Desktop\Grohe\Grohe\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{723CC480-C49A-42FE-93A7-566CCB4D2505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FFBB14-074B-4CC8-BC57-7C5594932DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="104">
   <si>
     <t>Заявка към доставчик  0000000464   20.01.2025</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Срок</t>
   </si>
   <si>
-    <t>157087</t>
-  </si>
-  <si>
     <t>29193AL1</t>
   </si>
   <si>
@@ -97,210 +94,111 @@
     <t/>
   </si>
   <si>
-    <t>2309</t>
-  </si>
-  <si>
-    <t>22025000</t>
-  </si>
-  <si>
     <t>СК ъглов 1/2-1/2 22025000 GROHE ПРОМО</t>
   </si>
   <si>
-    <t>159576</t>
-  </si>
-  <si>
-    <t>1017490000</t>
-  </si>
-  <si>
     <t>1017490000 Cubeo смесител за умивалник  M размер ПРОМО</t>
   </si>
   <si>
     <t>мостри Флайт Ел</t>
   </si>
   <si>
-    <t>159577</t>
-  </si>
-  <si>
-    <t>1017290000</t>
-  </si>
-  <si>
     <t>1017290000 Cubeo смесител за умивалник  XL размер ПРОМО</t>
   </si>
   <si>
     <t>мостри Флайт ЕЛ</t>
   </si>
   <si>
-    <t>159579</t>
-  </si>
-  <si>
-    <t>1017492430</t>
-  </si>
-  <si>
     <t>1017492430 Cubeo смесител за умивалник  M размер ПРОМО</t>
   </si>
   <si>
-    <t>159580</t>
-  </si>
-  <si>
-    <t>1017292430</t>
-  </si>
-  <si>
     <t>1017292430 Cubeo смесител за умивалник  XL размер ПРОМО</t>
   </si>
   <si>
-    <t>159581</t>
-  </si>
-  <si>
-    <t>1018130000</t>
-  </si>
-  <si>
     <t>1018130000 Cubeo смесител за вана /душ  ПРОМО</t>
   </si>
   <si>
     <t>мостра Флайт Ел</t>
   </si>
   <si>
-    <t>159583</t>
-  </si>
-  <si>
-    <t>1018132430</t>
-  </si>
-  <si>
     <t>1018132430 Cubeo смесител за вана /душ  ПРОМО</t>
   </si>
   <si>
-    <t>53686</t>
-  </si>
-  <si>
     <t>29509KF0</t>
   </si>
   <si>
     <t xml:space="preserve">29509KF0 Сифон бутилков за умивалник </t>
   </si>
   <si>
-    <t>53682</t>
-  </si>
-  <si>
     <t>41217KF0</t>
   </si>
   <si>
     <t>41217KF0 Selection държач за чаша/дозатор течен сапун ПРОМО</t>
   </si>
   <si>
-    <t>157676</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41029000 </t>
-  </si>
-  <si>
     <t>41029000 Selection Чаша ПРОМО</t>
   </si>
   <si>
-    <t>53683</t>
-  </si>
-  <si>
     <t>41218KF0</t>
   </si>
   <si>
     <t>41218KF0 Selection дозатор течен сапун ПРОМО</t>
   </si>
   <si>
-    <t>53687</t>
-  </si>
-  <si>
     <t>29510KF0</t>
   </si>
   <si>
     <t>29510KF0 Сифон push-open ПРОМО</t>
   </si>
   <si>
-    <t>53657</t>
-  </si>
-  <si>
     <t>22124KF0</t>
   </si>
   <si>
     <t>22124KF0 Rainshower SmarActive душ глава с рамо 142мм ПРОМО за тяло 26483000 или 26484000</t>
   </si>
   <si>
-    <t>53662</t>
-  </si>
-  <si>
     <t>29508KF0</t>
   </si>
   <si>
     <t>29508KF0 GRTSmarControl термостат за вграждане с 3 изхода ПРОМО</t>
   </si>
   <si>
-    <t>53643</t>
-  </si>
-  <si>
     <t>31892KF0</t>
   </si>
   <si>
     <t>31892KF0 Essence Smart Control издърпващ се L - чучур, 2 струи ПРОМО</t>
   </si>
   <si>
-    <t>53642</t>
-  </si>
-  <si>
     <t>31928KF0</t>
   </si>
   <si>
     <t>31928KF0 Essence Smart Control издърпващ се L - чучур ПРОМО</t>
   </si>
   <si>
-    <t>53640</t>
-  </si>
-  <si>
     <t>30504KF0</t>
   </si>
   <si>
     <t>30504KF0 Essence смесител за кухня стоящ издърпващ L чучур ПРОМО</t>
   </si>
   <si>
-    <t>53641</t>
-  </si>
-  <si>
     <t>30503KF0</t>
   </si>
   <si>
     <t>30503KF0 Essence смесител за кухня стоящ profi-spray ПРОМО</t>
   </si>
   <si>
-    <t>52190</t>
-  </si>
-  <si>
-    <t>38784000</t>
-  </si>
-  <si>
     <t>38784000 Skate Cosmopolitan за писоар</t>
   </si>
   <si>
-    <t>85194</t>
-  </si>
-  <si>
-    <t>19895000</t>
-  </si>
-  <si>
     <t>19895000 Eurocube двудупков смесител за умивалник стенен S размер</t>
   </si>
   <si>
-    <t>53138</t>
-  </si>
-  <si>
-    <t>49081000</t>
-  </si>
-  <si>
     <t>49081000 Ръкохватка</t>
   </si>
   <si>
     <t>Кристин</t>
   </si>
   <si>
-    <t>151313</t>
-  </si>
-  <si>
     <t>31580SD1</t>
   </si>
   <si>
@@ -310,228 +208,108 @@
     <t>Лотос 7 бр</t>
   </si>
   <si>
-    <t>159903</t>
-  </si>
-  <si>
-    <t>24272001</t>
-  </si>
-  <si>
     <t>24272001 EuroEco 2023 смесител за умивалник L размер ПРОМО</t>
   </si>
   <si>
     <t>мостра Айко Варна</t>
   </si>
   <si>
-    <t>157549</t>
-  </si>
-  <si>
     <t>2759730E</t>
   </si>
   <si>
     <t>2759730E Tempesta  110 II 5.7 l/min струи душ ръчен ПРОМО</t>
   </si>
   <si>
-    <t>157730</t>
-  </si>
-  <si>
-    <t>40778001</t>
-  </si>
-  <si>
     <t xml:space="preserve">40778001 Essentials Cube к-кт 4 в 1 </t>
   </si>
   <si>
-    <t>123166</t>
-  </si>
-  <si>
-    <t>19286001</t>
-  </si>
-  <si>
     <t>19286001 Essence New бутон за см. за вгр</t>
   </si>
   <si>
     <t>Гресия офис</t>
   </si>
   <si>
-    <t>159893</t>
-  </si>
-  <si>
-    <t>13449001</t>
-  </si>
-  <si>
     <t>13449001 Essence чучур за вана</t>
   </si>
   <si>
-    <t>159641</t>
-  </si>
-  <si>
-    <t>194502433</t>
-  </si>
-  <si>
     <t>194502433 Eurosmart смесител за враждане за вана /душ без тяло 33963 ПРОМО</t>
   </si>
   <si>
     <t>оферта 2810А</t>
   </si>
   <si>
-    <t>157565</t>
-  </si>
-  <si>
-    <t>267462433</t>
-  </si>
-  <si>
     <t>267462433 Tempesta Cube 110 II ръчен душ 9.5l ПРОМО</t>
   </si>
   <si>
-    <t>159600</t>
-  </si>
-  <si>
-    <t>286282431</t>
-  </si>
-  <si>
     <t>286282431 Tempesta стенно коляно ПРОМО</t>
   </si>
   <si>
-    <t>53663</t>
-  </si>
-  <si>
     <t>28362KF1</t>
   </si>
   <si>
     <t>28362KF1 Шлаух за душ 1250мм ПРОМО</t>
   </si>
   <si>
-    <t>159601</t>
-  </si>
-  <si>
-    <t>266872430</t>
-  </si>
-  <si>
     <t>266872430 NTempesta Cube 250 душ пита комплект с рамо ПРОМО</t>
   </si>
   <si>
-    <t>85850</t>
-  </si>
-  <si>
-    <t>33963000</t>
-  </si>
-  <si>
     <t>35501000 / 33963000 Rapido E универсален разпред. ПРОМО</t>
   </si>
   <si>
-    <t>85299</t>
-  </si>
-  <si>
     <t>27707AL0</t>
   </si>
   <si>
     <t>27707AL0 Allure Brilliant стенно коляно</t>
   </si>
   <si>
-    <t>157171</t>
-  </si>
-  <si>
-    <t>29192001</t>
-  </si>
-  <si>
     <t>29192001 / 19408001 Essence New двудупков смесител за умивалник М размер</t>
   </si>
   <si>
-    <t>123662</t>
-  </si>
-  <si>
-    <t>40658001</t>
-  </si>
-  <si>
     <t>40658001 Essentials Authentic тоал. четка</t>
   </si>
   <si>
-    <t>157105</t>
-  </si>
-  <si>
     <t>29192DA1</t>
   </si>
   <si>
     <t>29192DA1 Essence двудупков смесител за умивалник</t>
   </si>
   <si>
-    <t>52782</t>
-  </si>
-  <si>
-    <t>66791000</t>
-  </si>
-  <si>
     <t xml:space="preserve">66791000 Ревизионна кутия за 156 x 197 mm </t>
   </si>
   <si>
-    <t>52178</t>
-  </si>
-  <si>
     <t>37624SH0</t>
   </si>
   <si>
     <t>37624SH0 Arena Cosmopolitan бутон S</t>
   </si>
   <si>
-    <t>52177</t>
-  </si>
-  <si>
     <t>38732DA0</t>
   </si>
   <si>
     <t>38732DA0 Skate Cosmopolitan бутон</t>
   </si>
   <si>
-    <t>52223</t>
-  </si>
-  <si>
     <t>38844SH0</t>
   </si>
   <si>
     <t>38844SH0 Arena Cosmop. спусък за тоал. к.</t>
   </si>
   <si>
-    <t>52725</t>
-  </si>
-  <si>
-    <t>46107000</t>
-  </si>
-  <si>
     <t>46107000 Превключвател</t>
   </si>
   <si>
-    <t>157445</t>
-  </si>
-  <si>
-    <t>32757001</t>
-  </si>
-  <si>
     <t>32757001 Allure New смесител за умивалник М р-р</t>
   </si>
   <si>
     <t>Business partner</t>
   </si>
   <si>
-    <t>159898</t>
-  </si>
-  <si>
-    <t>24160001</t>
-  </si>
-  <si>
     <t>24160001 Allure New смесител за биде</t>
   </si>
   <si>
-    <t>157018</t>
-  </si>
-  <si>
-    <t>34870000</t>
-  </si>
-  <si>
     <t xml:space="preserve">34870000 Grohtherm Rainshower Mono 310 душ система ПРОМО </t>
   </si>
   <si>
-    <t>157415</t>
-  </si>
-  <si>
     <t>30590KF0</t>
   </si>
   <si>
@@ -539,12 +317,6 @@
   </si>
   <si>
     <t>Friends</t>
-  </si>
-  <si>
-    <t>151236</t>
-  </si>
-  <si>
-    <t>39125001</t>
   </si>
   <si>
     <t>39125001 Eurosmart  умивалник за вграждане под  плот</t>
@@ -608,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -625,16 +397,19 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -650,9 +425,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Оffice">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -690,7 +465,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Оffice">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -796,7 +571,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Оffice">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -948,14 +723,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:K10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="7"/>
@@ -972,7 +747,7 @@
       <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+      <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -987,7 +762,7 @@
       <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="7"/>
@@ -1004,7 +779,7 @@
       <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1019,7 +794,7 @@
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="7"/>
@@ -1036,7 +811,7 @@
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="7"/>
@@ -1053,7 +828,7 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="7"/>
@@ -1070,7 +845,7 @@
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -1126,20 +901,20 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="9">
+        <v>157087</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F10" s="3">
         <v>320.96800100000002</v>
@@ -1151,36 +926,36 @@
         <v>0</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J10" s="4">
         <v>320.96800100000002</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L10" s="4">
         <v>320.96800100000002</v>
       </c>
       <c r="M10" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>2309</v>
+      </c>
+      <c r="B11" s="9">
+        <v>22025000</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D11" s="3">
         <v>100</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="3">
         <v>3.7160769999999999</v>
@@ -1192,7 +967,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J11" s="4">
         <v>371.60770000000002</v>
@@ -1202,24 +977,24 @@
         <v>371.60770000000002</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>29</v>
+      <c r="A12" s="9">
+        <v>159576</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1017490000</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D12" s="3">
         <v>3</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="3">
         <v>62.537663999999999</v>
@@ -1231,36 +1006,36 @@
         <v>0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J12" s="4">
         <v>187.61299199999999</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="L12" s="4">
         <v>187.61299199999999</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>33</v>
+      <c r="A13" s="9">
+        <v>159577</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1017290000</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D13" s="3">
         <v>3</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F13" s="3">
         <v>130.307174</v>
@@ -1272,36 +1047,36 @@
         <v>0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J13" s="4">
         <v>390.92152199999998</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="L13" s="4">
         <v>390.92152199999998</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>37</v>
+      <c r="A14" s="9">
+        <v>159579</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1017492430</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3">
         <v>3</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F14" s="3">
         <v>81.297334000000006</v>
@@ -1313,36 +1088,36 @@
         <v>0</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J14" s="4">
         <v>243.89200199999999</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="L14" s="4">
         <v>243.89200199999999</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>40</v>
+      <c r="A15" s="9">
+        <v>159580</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1017292430</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D15" s="3">
         <v>3</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="3">
         <v>115.247283</v>
@@ -1354,36 +1129,36 @@
         <v>0</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J15" s="4">
         <v>345.741849</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="L15" s="4">
         <v>345.741849</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>43</v>
+      <c r="A16" s="9">
+        <v>159581</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1018130000</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D16" s="3">
         <v>3</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F16" s="3">
         <v>65.259528000000003</v>
@@ -1395,36 +1170,36 @@
         <v>0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J16" s="4">
         <v>195.778584</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="L16" s="4">
         <v>195.778584</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>47</v>
+      <c r="A17" s="9">
+        <v>159583</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1018132430</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D17" s="3">
         <v>3</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F17" s="3">
         <v>84.834125999999998</v>
@@ -1436,36 +1211,36 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J17" s="4">
         <v>254.50237799999999</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="L17" s="4">
         <v>254.50237799999999</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>49</v>
+      <c r="A18" s="9">
+        <v>53686</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3">
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F18" s="3">
         <v>87.490795000000006</v>
@@ -1477,7 +1252,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J18" s="4">
         <v>874.90795000000003</v>
@@ -1487,24 +1262,24 @@
         <v>874.90795000000003</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>52</v>
+      <c r="A19" s="9">
+        <v>53682</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D19" s="3">
         <v>20</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F19" s="3">
         <v>44.152861999999999</v>
@@ -1516,7 +1291,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J19" s="4">
         <v>883.05723999999998</v>
@@ -1526,24 +1301,24 @@
         <v>883.05723999999998</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>56</v>
+      <c r="A20" s="9">
+        <v>157676</v>
+      </c>
+      <c r="B20" s="9">
+        <v>41029000</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D20" s="3">
         <v>20</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="3">
         <v>22.166073000000001</v>
@@ -1555,7 +1330,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J20" s="4">
         <v>443.32146</v>
@@ -1565,24 +1340,24 @@
         <v>443.32146</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>58</v>
+      <c r="A21" s="9">
+        <v>53683</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D21" s="3">
         <v>20</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F21" s="3">
         <v>44.152861999999999</v>
@@ -1594,7 +1369,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J21" s="4">
         <v>883.05723999999998</v>
@@ -1604,24 +1379,24 @@
         <v>883.05723999999998</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>61</v>
+      <c r="A22" s="9">
+        <v>53687</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D22" s="3">
         <v>20</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F22" s="3">
         <v>43.598711000000002</v>
@@ -1633,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J22" s="4">
         <v>871.97421999999995</v>
@@ -1643,24 +1418,24 @@
         <v>871.97421999999995</v>
       </c>
       <c r="M22" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>64</v>
+      <c r="A23" s="9">
+        <v>53657</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="D23" s="3">
         <v>20</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F23" s="3">
         <v>488.32185500000003</v>
@@ -1672,7 +1447,7 @@
         <v>0</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J23" s="4">
         <v>9766.4370999999992</v>
@@ -1682,24 +1457,24 @@
         <v>9766.4370999999992</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>67</v>
+      <c r="A24" s="9">
+        <v>53662</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="D24" s="3">
         <v>10</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F24" s="3">
         <v>550.64763900000003</v>
@@ -1711,7 +1486,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J24" s="4">
         <v>5506.4763899999998</v>
@@ -1721,24 +1496,24 @@
         <v>5506.4763899999998</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>70</v>
+      <c r="A25" s="9">
+        <v>53643</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="D25" s="3">
         <v>10</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F25" s="3">
         <v>622.76886999999999</v>
@@ -1750,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J25" s="4">
         <v>6227.6886999999997</v>
@@ -1760,24 +1535,24 @@
         <v>6227.6886999999997</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>73</v>
+      <c r="A26" s="9">
+        <v>53642</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D26" s="3">
         <v>10</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F26" s="3">
         <v>376.05721299999999</v>
@@ -1789,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J26" s="4">
         <v>3760.57213</v>
@@ -1799,24 +1574,24 @@
         <v>3760.57213</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>76</v>
+      <c r="A27" s="9">
+        <v>53640</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D27" s="3">
         <v>10</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F27" s="3">
         <v>348.03994899999998</v>
@@ -1828,7 +1603,7 @@
         <v>0</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J27" s="4">
         <v>3480.3994899999998</v>
@@ -1838,24 +1613,24 @@
         <v>3480.3994899999998</v>
       </c>
       <c r="M27" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>79</v>
+      <c r="A28" s="9">
+        <v>53641</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="D28" s="3">
         <v>10</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F28" s="3">
         <v>492.91805599999998</v>
@@ -1867,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J28" s="4">
         <v>4929.1805599999998</v>
@@ -1877,24 +1652,24 @@
         <v>4929.1805599999998</v>
       </c>
       <c r="M28" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>83</v>
+      <c r="A29" s="9">
+        <v>52190</v>
+      </c>
+      <c r="B29" s="9">
+        <v>38784000</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="D29" s="3">
         <v>5</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F29" s="3">
         <v>106.560137</v>
@@ -1906,7 +1681,7 @@
         <v>0</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J29" s="4">
         <v>532.80068500000004</v>
@@ -1916,24 +1691,24 @@
         <v>532.80068500000004</v>
       </c>
       <c r="M29" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>86</v>
+      <c r="A30" s="9">
+        <v>85194</v>
+      </c>
+      <c r="B30" s="9">
+        <v>19895000</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="D30" s="3">
         <v>10</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F30" s="3">
         <v>226.41991999999999</v>
@@ -1945,7 +1720,7 @@
         <v>0</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J30" s="4">
         <v>2264.1992</v>
@@ -1955,24 +1730,24 @@
         <v>2264.1992</v>
       </c>
       <c r="M30" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>89</v>
+      <c r="A31" s="9">
+        <v>53138</v>
+      </c>
+      <c r="B31" s="9">
+        <v>49081000</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="D31" s="3">
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F31" s="3">
         <v>25.914747999999999</v>
@@ -1984,36 +1759,36 @@
         <v>0</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J31" s="4">
         <v>51.829495999999999</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="L31" s="4">
         <v>51.829495999999999</v>
       </c>
       <c r="M31" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>92</v>
+      <c r="A32" s="9">
+        <v>151313</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="D32" s="3">
         <v>16</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F32" s="3">
         <v>258.07176900000002</v>
@@ -2025,36 +1800,36 @@
         <v>0</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J32" s="4">
         <v>4129.1483040000003</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="L32" s="4">
         <v>4129.1483040000003</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>97</v>
+      <c r="A33" s="9">
+        <v>159903</v>
+      </c>
+      <c r="B33" s="9">
+        <v>24272001</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="D33" s="3">
         <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F33" s="3">
         <v>54.616553000000003</v>
@@ -2066,36 +1841,36 @@
         <v>0</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J33" s="4">
         <v>54.616553000000003</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="L33" s="4">
         <v>54.616553000000003</v>
       </c>
       <c r="M33" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>100</v>
+      <c r="A34" s="9">
+        <v>157549</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="D34" s="3">
         <v>50</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F34" s="3">
         <v>15.972612</v>
@@ -2107,7 +1882,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J34" s="4">
         <v>798.63059999999996</v>
@@ -2117,24 +1892,24 @@
         <v>798.63059999999996</v>
       </c>
       <c r="M34" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>104</v>
+      <c r="A35" s="9">
+        <v>157730</v>
+      </c>
+      <c r="B35" s="9">
+        <v>40778001</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
       <c r="D35" s="3">
         <v>5</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F35" s="3">
         <v>111.02500000000001</v>
@@ -2146,7 +1921,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J35" s="4">
         <v>555.125</v>
@@ -2156,24 +1931,24 @@
         <v>555.125</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>107</v>
+      <c r="A36" s="9">
+        <v>123166</v>
+      </c>
+      <c r="B36" s="9">
+        <v>19286001</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="D36" s="3">
         <v>1</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F36" s="3">
         <v>152.75</v>
@@ -2185,36 +1960,36 @@
         <v>0</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J36" s="4">
         <v>152.75</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="L36" s="4">
         <v>152.75</v>
       </c>
       <c r="M36" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>111</v>
+      <c r="A37" s="9">
+        <v>159893</v>
+      </c>
+      <c r="B37" s="9">
+        <v>13449001</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>112</v>
+        <v>69</v>
       </c>
       <c r="D37" s="3">
         <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F37" s="3">
         <v>105.223654</v>
@@ -2226,36 +2001,36 @@
         <v>0</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J37" s="4">
         <v>105.223654</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="L37" s="4">
         <v>105.223654</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>114</v>
+      <c r="A38" s="9">
+        <v>159641</v>
+      </c>
+      <c r="B38" s="9">
+        <v>194502433</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>115</v>
+        <v>70</v>
       </c>
       <c r="D38" s="3">
         <v>132</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F38" s="3">
         <v>84.491855999999999</v>
@@ -2267,36 +2042,36 @@
         <v>0</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J38" s="4">
         <v>11152.924992</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="L38" s="4">
         <v>11152.924992</v>
       </c>
       <c r="M38" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>118</v>
+      <c r="A39" s="9">
+        <v>157565</v>
+      </c>
+      <c r="B39" s="9">
+        <v>267462433</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>119</v>
+        <v>72</v>
       </c>
       <c r="D39" s="3">
         <v>132</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F39" s="3">
         <v>23.372169</v>
@@ -2308,36 +2083,36 @@
         <v>0</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J39" s="4">
         <v>3085.1263079999999</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="L39" s="4">
         <v>3085.1263079999999</v>
       </c>
       <c r="M39" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>121</v>
+      <c r="A40" s="9">
+        <v>159600</v>
+      </c>
+      <c r="B40" s="9">
+        <v>286282431</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
       <c r="D40" s="3">
         <v>132</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F40" s="3">
         <v>32.662360999999997</v>
@@ -2349,36 +2124,36 @@
         <v>0</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J40" s="4">
         <v>4311.4316520000002</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="L40" s="4">
         <v>4311.4316520000002</v>
       </c>
       <c r="M40" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>123</v>
+      <c r="A41" s="9">
+        <v>53663</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="D41" s="3">
         <v>132</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F41" s="3">
         <v>19.444210999999999</v>
@@ -2390,36 +2165,36 @@
         <v>0</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J41" s="4">
         <v>2566.6358519999999</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="L41" s="4">
         <v>2566.6358519999999</v>
       </c>
       <c r="M41" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>127</v>
+      <c r="A42" s="9">
+        <v>159601</v>
+      </c>
+      <c r="B42" s="9">
+        <v>266872430</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="D42" s="3">
         <v>132</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F42" s="3">
         <v>190.66082700000001</v>
@@ -2431,36 +2206,36 @@
         <v>0</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J42" s="4">
         <v>25167.229164</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="L42" s="4">
         <v>25167.229164</v>
       </c>
       <c r="M42" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>130</v>
+      <c r="A43" s="9">
+        <v>85850</v>
+      </c>
+      <c r="B43" s="9">
+        <v>33963000</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="D43" s="3">
         <v>132</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F43" s="3">
         <v>59</v>
@@ -2472,36 +2247,36 @@
         <v>0</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J43" s="4">
         <v>7788</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="L43" s="4">
         <v>7788</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>132</v>
+      <c r="A44" s="9">
+        <v>85299</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>133</v>
+        <v>78</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>134</v>
+        <v>79</v>
       </c>
       <c r="D44" s="3">
         <v>5</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F44" s="3">
         <v>56.604981000000002</v>
@@ -2513,7 +2288,7 @@
         <v>0</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J44" s="4">
         <v>283.02490499999999</v>
@@ -2523,24 +2298,24 @@
         <v>283.02490499999999</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>136</v>
+      <c r="A45" s="9">
+        <v>157171</v>
+      </c>
+      <c r="B45" s="9">
+        <v>29192001</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>137</v>
+        <v>80</v>
       </c>
       <c r="D45" s="3">
         <v>10</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F45" s="3">
         <v>178.06202400000001</v>
@@ -2552,7 +2327,7 @@
         <v>0</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J45" s="4">
         <v>1780.62024</v>
@@ -2562,24 +2337,24 @@
         <v>1780.62024</v>
       </c>
       <c r="M45" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>139</v>
+      <c r="A46" s="9">
+        <v>123662</v>
+      </c>
+      <c r="B46" s="9">
+        <v>40658001</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>140</v>
+        <v>81</v>
       </c>
       <c r="D46" s="3">
         <v>5</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F46" s="3">
         <v>38.33</v>
@@ -2591,7 +2366,7 @@
         <v>0</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J46" s="4">
         <v>191.65</v>
@@ -2601,24 +2376,24 @@
         <v>191.65</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>141</v>
+      <c r="A47" s="9">
+        <v>157105</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>142</v>
+        <v>82</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
       <c r="D47" s="3">
         <v>5</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F47" s="3">
         <v>214.48935700000001</v>
@@ -2630,7 +2405,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J47" s="4">
         <v>1072.4467850000001</v>
@@ -2640,24 +2415,24 @@
         <v>1072.4467850000001</v>
       </c>
       <c r="M47" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>145</v>
+      <c r="A48" s="9">
+        <v>52782</v>
+      </c>
+      <c r="B48" s="9">
+        <v>66791000</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="D48" s="3">
         <v>20</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F48" s="3">
         <v>8.7849369999999993</v>
@@ -2669,7 +2444,7 @@
         <v>0</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J48" s="4">
         <v>175.69873999999999</v>
@@ -2679,24 +2454,24 @@
         <v>175.69873999999999</v>
       </c>
       <c r="M48" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
-        <v>147</v>
+      <c r="A49" s="9">
+        <v>52178</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>148</v>
+        <v>85</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="D49" s="3">
         <v>5</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F49" s="3">
         <v>64.786868999999996</v>
@@ -2708,7 +2483,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J49" s="4">
         <v>323.93434500000001</v>
@@ -2718,24 +2493,24 @@
         <v>323.93434500000001</v>
       </c>
       <c r="M49" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>150</v>
+      <c r="A50" s="9">
+        <v>52177</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>152</v>
+        <v>88</v>
       </c>
       <c r="D50" s="3">
         <v>5</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F50" s="3">
         <v>120.870294</v>
@@ -2747,7 +2522,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J50" s="4">
         <v>604.35146999999995</v>
@@ -2757,24 +2532,24 @@
         <v>604.35146999999995</v>
       </c>
       <c r="M50" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>153</v>
+      <c r="A51" s="9">
+        <v>52223</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>154</v>
+        <v>89</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>155</v>
+        <v>90</v>
       </c>
       <c r="D51" s="3">
         <v>5</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F51" s="3">
         <v>51.177551999999999</v>
@@ -2786,7 +2561,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J51" s="4">
         <v>255.88775999999999</v>
@@ -2796,24 +2571,24 @@
         <v>255.88775999999999</v>
       </c>
       <c r="M51" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>157</v>
+      <c r="A52" s="9">
+        <v>52725</v>
+      </c>
+      <c r="B52" s="9">
+        <v>46107000</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="D52" s="3">
         <v>3</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F52" s="3">
         <v>21.986789999999999</v>
@@ -2825,7 +2600,7 @@
         <v>0</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J52" s="4">
         <v>65.960369999999998</v>
@@ -2835,24 +2610,24 @@
         <v>65.960369999999998</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>160</v>
+      <c r="A53" s="9">
+        <v>157445</v>
+      </c>
+      <c r="B53" s="9">
+        <v>32757001</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>161</v>
+        <v>92</v>
       </c>
       <c r="D53" s="3">
         <v>1</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F53" s="3">
         <v>0</v>
@@ -2864,36 +2639,36 @@
         <v>0</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J53" s="4">
         <v>0</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>162</v>
+        <v>93</v>
       </c>
       <c r="L53" s="4">
         <v>0</v>
       </c>
       <c r="M53" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>164</v>
+      <c r="A54" s="9">
+        <v>159898</v>
+      </c>
+      <c r="B54" s="9">
+        <v>24160001</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
       <c r="D54" s="3">
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F54" s="3">
         <v>0</v>
@@ -2905,36 +2680,36 @@
         <v>0</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J54" s="4">
         <v>0</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>162</v>
+        <v>93</v>
       </c>
       <c r="L54" s="4">
         <v>0</v>
       </c>
       <c r="M54" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>167</v>
+      <c r="A55" s="9">
+        <v>157018</v>
+      </c>
+      <c r="B55" s="9">
+        <v>34870000</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>168</v>
+        <v>95</v>
       </c>
       <c r="D55" s="3">
         <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F55" s="3">
         <v>631.63529900000003</v>
@@ -2946,36 +2721,36 @@
         <v>0</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J55" s="4">
         <v>631.63529900000003</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>162</v>
+        <v>93</v>
       </c>
       <c r="L55" s="4">
         <v>631.63529900000003</v>
       </c>
       <c r="M55" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>169</v>
+      <c r="A56" s="9">
+        <v>157415</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>170</v>
+        <v>96</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>171</v>
+        <v>97</v>
       </c>
       <c r="D56" s="3">
         <v>1</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F56" s="3">
         <v>202.656586</v>
@@ -2987,36 +2762,36 @@
         <v>0</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J56" s="4">
         <v>202.656586</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>172</v>
+        <v>98</v>
       </c>
       <c r="L56" s="4">
         <v>202.656586</v>
       </c>
       <c r="M56" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>174</v>
+      <c r="A57" s="9">
+        <v>151236</v>
+      </c>
+      <c r="B57" s="9">
+        <v>39125001</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>175</v>
+        <v>99</v>
       </c>
       <c r="D57" s="3">
         <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F57" s="3">
         <v>110.634784</v>
@@ -3028,23 +2803,23 @@
         <v>0</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J57" s="4">
         <v>110.634784</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>176</v>
+        <v>100</v>
       </c>
       <c r="L57" s="4">
         <v>110.634784</v>
       </c>
       <c r="M57" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="8"/>
+      <c r="A58" s="6"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
@@ -3059,8 +2834,8 @@
       <c r="M58" s="7"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
-        <v>177</v>
+      <c r="A59" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -3076,8 +2851,8 @@
       <c r="M59" s="7"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="8" t="s">
-        <v>178</v>
+      <c r="A60" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -3093,8 +2868,8 @@
       <c r="M60" s="7"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="8" t="s">
-        <v>179</v>
+      <c r="A61" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -3111,6 +2886,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A5:M5"/>
     <mergeCell ref="A60:M60"/>
     <mergeCell ref="A61:M61"/>
     <mergeCell ref="A6:M6"/>
@@ -3118,11 +2898,6 @@
     <mergeCell ref="A8:M8"/>
     <mergeCell ref="A58:M58"/>
     <mergeCell ref="A59:M59"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="A5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Create reader for xlsx and make Pre Order.
</commit_message>
<xml_diff>
--- a/Grohe/src/main/resources/test.xlsx
+++ b/Grohe/src/main/resources/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T480s\Desktop\Grohe\Grohe\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Office\OneDrive\Desktop\Grohe orders\Grohe\Grohe\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57FFBB14-074B-4CC8-BC57-7C5594932DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2054EA16-97A2-4B2E-814C-61E69759F08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17835" yWindow="0" windowWidth="10335" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -380,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -397,6 +397,15 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -404,12 +413,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -425,9 +431,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Оffice">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -465,7 +471,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Оffice">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -571,7 +577,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Оffice">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -723,141 +729,144 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -869,7 +878,7 @@
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -901,7 +910,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="6">
         <v>157087</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -910,7 +919,7 @@
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="8">
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -942,16 +951,16 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="6">
         <v>2309</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="6">
         <v>22025000</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="8">
         <v>100</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -981,16 +990,16 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="6">
         <v>159576</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="6">
         <v>1017490000</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="8">
         <v>3</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1022,16 +1031,16 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="6">
         <v>159577</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="6">
         <v>1017290000</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="8">
         <v>3</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -1063,16 +1072,16 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="6">
         <v>159579</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="6">
         <v>1017492430</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="8">
         <v>3</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -1104,16 +1113,16 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="6">
         <v>159580</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="6">
         <v>1017292430</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="8">
         <v>3</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -1145,16 +1154,16 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="6">
         <v>159581</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="6">
         <v>1018130000</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="8">
         <v>3</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1186,16 +1195,16 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="6">
         <v>159583</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="6">
         <v>1018132430</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="8">
         <v>3</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1227,7 +1236,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="6">
         <v>53686</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1236,7 +1245,7 @@
       <c r="C18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="8">
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1266,7 +1275,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="6">
         <v>53682</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1275,7 +1284,7 @@
       <c r="C19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="8">
         <v>20</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -1305,16 +1314,16 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="A20" s="6">
         <v>157676</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="6">
         <v>41029000</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="8">
         <v>20</v>
       </c>
       <c r="E20" s="2" t="s">
@@ -1344,7 +1353,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="6">
         <v>53683</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1353,7 +1362,7 @@
       <c r="C21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="8">
         <v>20</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -1383,7 +1392,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="6">
         <v>53687</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1392,7 +1401,7 @@
       <c r="C22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="8">
         <v>20</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -1422,7 +1431,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="6">
         <v>53657</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1431,7 +1440,7 @@
       <c r="C23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="8">
         <v>20</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -1461,7 +1470,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="A24" s="6">
         <v>53662</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1470,7 +1479,7 @@
       <c r="C24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="8">
         <v>10</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -1500,7 +1509,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="A25" s="6">
         <v>53643</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1509,7 +1518,7 @@
       <c r="C25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="8">
         <v>10</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -1539,7 +1548,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="A26" s="6">
         <v>53642</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1548,7 +1557,7 @@
       <c r="C26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="8">
         <v>10</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -1578,7 +1587,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="6">
         <v>53640</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1587,7 +1596,7 @@
       <c r="C27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="8">
         <v>10</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -1617,7 +1626,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="A28" s="6">
         <v>53641</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1626,7 +1635,7 @@
       <c r="C28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="8">
         <v>10</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -1656,16 +1665,16 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="6">
         <v>52190</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="6">
         <v>38784000</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="8">
         <v>5</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -1695,16 +1704,16 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="A30" s="6">
         <v>85194</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="6">
         <v>19895000</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="8">
         <v>10</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -1734,16 +1743,16 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="A31" s="6">
         <v>53138</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="6">
         <v>49081000</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="8">
         <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -1775,7 +1784,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="A32" s="6">
         <v>151313</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1784,7 +1793,7 @@
       <c r="C32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="8">
         <v>16</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -1816,16 +1825,16 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="A33" s="6">
         <v>159903</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="6">
         <v>24272001</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="8">
         <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -1857,7 +1866,7 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+      <c r="A34" s="6">
         <v>157549</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1866,7 +1875,7 @@
       <c r="C34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="8">
         <v>50</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -1896,16 +1905,16 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="A35" s="6">
         <v>157730</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="6">
         <v>40778001</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="8">
         <v>5</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -1935,16 +1944,16 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+      <c r="A36" s="6">
         <v>123166</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="6">
         <v>19286001</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="8">
         <v>1</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -1976,16 +1985,16 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+      <c r="A37" s="6">
         <v>159893</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="6">
         <v>13449001</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="8">
         <v>1</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -2017,16 +2026,16 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+      <c r="A38" s="6">
         <v>159641</v>
       </c>
-      <c r="B38" s="9">
+      <c r="B38" s="6">
         <v>194502433</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="8">
         <v>132</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -2058,16 +2067,16 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="A39" s="6">
         <v>157565</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="6">
         <v>267462433</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="8">
         <v>132</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -2099,16 +2108,16 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+      <c r="A40" s="6">
         <v>159600</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="6">
         <v>286282431</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="8">
         <v>132</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -2140,7 +2149,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+      <c r="A41" s="6">
         <v>53663</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2149,7 +2158,7 @@
       <c r="C41" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="8">
         <v>132</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -2181,16 +2190,16 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+      <c r="A42" s="6">
         <v>159601</v>
       </c>
-      <c r="B42" s="9">
+      <c r="B42" s="6">
         <v>266872430</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="8">
         <v>132</v>
       </c>
       <c r="E42" s="2" t="s">
@@ -2222,16 +2231,16 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+      <c r="A43" s="6">
         <v>85850</v>
       </c>
-      <c r="B43" s="9">
+      <c r="B43" s="6">
         <v>33963000</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="8">
         <v>132</v>
       </c>
       <c r="E43" s="2" t="s">
@@ -2263,7 +2272,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="9">
+      <c r="A44" s="6">
         <v>85299</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -2272,7 +2281,7 @@
       <c r="C44" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="8">
         <v>5</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -2302,16 +2311,16 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="9">
+      <c r="A45" s="6">
         <v>157171</v>
       </c>
-      <c r="B45" s="9">
+      <c r="B45" s="6">
         <v>29192001</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="8">
         <v>10</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -2341,16 +2350,16 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="9">
+      <c r="A46" s="6">
         <v>123662</v>
       </c>
-      <c r="B46" s="9">
+      <c r="B46" s="6">
         <v>40658001</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="8">
         <v>5</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -2380,7 +2389,7 @@
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="9">
+      <c r="A47" s="6">
         <v>157105</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -2389,7 +2398,7 @@
       <c r="C47" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="8">
         <v>5</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -2419,16 +2428,16 @@
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="9">
+      <c r="A48" s="6">
         <v>52782</v>
       </c>
-      <c r="B48" s="9">
+      <c r="B48" s="6">
         <v>66791000</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="8">
         <v>20</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -2458,7 +2467,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" s="9">
+      <c r="A49" s="6">
         <v>52178</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -2467,7 +2476,7 @@
       <c r="C49" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="8">
         <v>5</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -2497,7 +2506,7 @@
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="9">
+      <c r="A50" s="6">
         <v>52177</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2506,7 +2515,7 @@
       <c r="C50" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="8">
         <v>5</v>
       </c>
       <c r="E50" s="2" t="s">
@@ -2536,7 +2545,7 @@
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" s="9">
+      <c r="A51" s="6">
         <v>52223</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -2545,7 +2554,7 @@
       <c r="C51" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="8">
         <v>5</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -2575,16 +2584,16 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="9">
+      <c r="A52" s="6">
         <v>52725</v>
       </c>
-      <c r="B52" s="9">
+      <c r="B52" s="6">
         <v>46107000</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="8">
         <v>3</v>
       </c>
       <c r="E52" s="2" t="s">
@@ -2614,16 +2623,16 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" s="9">
+      <c r="A53" s="6">
         <v>157445</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B53" s="6">
         <v>32757001</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="8">
         <v>1</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -2655,16 +2664,16 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="9">
+      <c r="A54" s="6">
         <v>159898</v>
       </c>
-      <c r="B54" s="9">
+      <c r="B54" s="6">
         <v>24160001</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="8">
         <v>1</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -2696,16 +2705,16 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="9">
+      <c r="A55" s="6">
         <v>157018</v>
       </c>
-      <c r="B55" s="9">
+      <c r="B55" s="6">
         <v>34870000</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="8">
         <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -2737,7 +2746,7 @@
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A56" s="9">
+      <c r="A56" s="6">
         <v>157415</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -2746,7 +2755,7 @@
       <c r="C56" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="8">
         <v>1</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -2778,16 +2787,16 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="9">
+      <c r="A57" s="6">
         <v>151236</v>
       </c>
-      <c r="B57" s="9">
+      <c r="B57" s="6">
         <v>39125001</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="8">
         <v>1</v>
       </c>
       <c r="E57" s="2" t="s">
@@ -2819,70 +2828,70 @@
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="6"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
-      <c r="I58" s="7"/>
-      <c r="J58" s="7"/>
-      <c r="K58" s="7"/>
-      <c r="L58" s="7"/>
-      <c r="M58" s="7"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="10"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+      <c r="M59" s="10"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7"/>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7"/>
-      <c r="I60" s="7"/>
-      <c r="J60" s="7"/>
-      <c r="K60" s="7"/>
-      <c r="L60" s="7"/>
-      <c r="M60" s="7"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="10"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-      <c r="I61" s="7"/>
-      <c r="J61" s="7"/>
-      <c r="K61" s="7"/>
-      <c r="L61" s="7"/>
-      <c r="M61" s="7"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
+      <c r="M61" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>